<commit_message>
SW - config - ethernet devices added
</commit_message>
<xml_diff>
--- a/RF-Lab_Device-List.xlsx
+++ b/RF-Lab_Device-List.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Device List" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Device List'!$A$1:$O$39</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Device List'!$A$1:$P$39</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="115">
   <si>
     <t>USB-Vendor-ID</t>
   </si>
@@ -339,6 +339,63 @@
   </si>
   <si>
     <t>old</t>
+  </si>
+  <si>
+    <t>HFT  IP address</t>
+  </si>
+  <si>
+    <t>141.19.89.142</t>
+  </si>
+  <si>
+    <t>141.19.89.143</t>
+  </si>
+  <si>
+    <t>141.19.89.221</t>
+  </si>
+  <si>
+    <t>141.19.89.222</t>
+  </si>
+  <si>
+    <t>141.19.89.223</t>
+  </si>
+  <si>
+    <t>141.19.89.224</t>
+  </si>
+  <si>
+    <t>141.19.89.225</t>
+  </si>
+  <si>
+    <t>141.19.89.226</t>
+  </si>
+  <si>
+    <t>141.19.89.227</t>
+  </si>
+  <si>
+    <t>141.19.89.228</t>
+  </si>
+  <si>
+    <t>141.19.89.229</t>
+  </si>
+  <si>
+    <t>141.19.89.230</t>
+  </si>
+  <si>
+    <t>141.19.89.152</t>
+  </si>
+  <si>
+    <t>141.19.89.151</t>
+  </si>
+  <si>
+    <t>141.19.89.141</t>
+  </si>
+  <si>
+    <t>141.19.89.163, 141.19.89.164</t>
+  </si>
+  <si>
+    <t>141.19.89.161</t>
+  </si>
+  <si>
+    <t>141.19.89.162</t>
   </si>
 </sst>
 </file>
@@ -586,7 +643,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -609,9 +666,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -699,10 +753,16 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -983,10 +1043,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q39"/>
+  <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,17 +1056,17 @@
     <col min="3" max="3" width="5.7109375" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" customWidth="1"/>
-    <col min="8" max="9" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="7" customWidth="1"/>
-    <col min="11" max="11" width="5.7109375" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" customWidth="1"/>
-    <col min="13" max="13" width="5.7109375" customWidth="1"/>
-    <col min="14" max="15" width="8.7109375" customWidth="1"/>
+    <col min="6" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" customWidth="1"/>
+    <col min="9" max="10" width="14.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="7" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" customWidth="1"/>
+    <col min="14" max="14" width="5.7109375" customWidth="1"/>
+    <col min="15" max="16" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="90" t="s">
         <v>86</v>
       </c>
@@ -1024,1114 +1084,1202 @@
       <c r="M1" s="90"/>
       <c r="N1" s="90"/>
       <c r="O1" s="90"/>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="70" t="s">
+      <c r="P1" s="90"/>
+    </row>
+    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="70" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="58" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="23" t="s">
+      <c r="G3" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" s="11"/>
+      <c r="I3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="J3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="K3" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="11"/>
+      <c r="M3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="12"/>
-      <c r="N3" s="23" t="s">
+      <c r="N3" s="12"/>
+      <c r="O3" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="O3" s="50" t="s">
+      <c r="P3" s="49" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="72"/>
-      <c r="B4" s="73"/>
-      <c r="D4" s="60"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="51"/>
-    </row>
-    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="74" t="s">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="71"/>
+      <c r="B4" s="72"/>
+      <c r="D4" s="59"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="50"/>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="74" t="s">
         <v>35</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="61" t="s">
+      <c r="D5" s="60" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="29" t="s">
+      <c r="F5" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="30" t="s">
+      <c r="J5" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="31" t="s">
+      <c r="K5" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="4"/>
+      <c r="M5" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="4"/>
-      <c r="N5" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="O5" s="52" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="76"/>
-      <c r="B6" s="77"/>
-      <c r="D6" s="62"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="51"/>
-    </row>
-    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="78" t="s">
+      <c r="N5" s="4"/>
+      <c r="O5" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="P5" s="51" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="75"/>
+      <c r="B6" s="76"/>
+      <c r="D6" s="61"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="50"/>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="78" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="9"/>
-      <c r="D7" s="63" t="s">
+      <c r="D7" s="62" t="s">
         <v>26</v>
       </c>
       <c r="E7" s="9"/>
-      <c r="F7" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="32" t="s">
+      <c r="F7" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="J7" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="34" t="s">
+      <c r="K7" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="M7" s="9"/>
-      <c r="N7" s="32" t="s">
+      <c r="L7" s="9"/>
+      <c r="M7" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="N7" s="9"/>
+      <c r="O7" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="O7" s="53" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="76"/>
-      <c r="B8" s="77"/>
-      <c r="D8" s="62"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="51"/>
-    </row>
-    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="80" t="s">
+      <c r="P7" s="52" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="75"/>
+      <c r="B8" s="76"/>
+      <c r="D8" s="61"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="50"/>
+    </row>
+    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="81" t="s">
+      <c r="B9" s="80" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="6"/>
-      <c r="D9" s="64" t="s">
+      <c r="D9" s="63" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="35" t="s">
+      <c r="G9" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="I9" s="36" t="s">
+      <c r="J9" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="37">
+      <c r="K9" s="36">
         <v>3</v>
       </c>
-      <c r="K9" s="6"/>
-      <c r="L9" s="17" t="s">
+      <c r="L9" s="6"/>
+      <c r="M9" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="M9" s="6"/>
-      <c r="N9" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="O9" s="54" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="80" t="s">
+      <c r="N9" s="6"/>
+      <c r="O9" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P9" s="53" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="81" t="s">
+      <c r="B10" s="80" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="6"/>
-      <c r="D10" s="64" t="s">
+      <c r="D10" s="63" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="6"/>
-      <c r="F10" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="K10" s="6"/>
-      <c r="L10" s="17" t="s">
+      <c r="F10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" s="6"/>
+      <c r="M10" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="M10" s="6"/>
-      <c r="N10" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="O10" s="54" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q10" s="91" t="s">
+      <c r="N10" s="6"/>
+      <c r="O10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P10" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="R10" s="89" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="80" t="s">
+    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="80" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="6"/>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="63" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="35" t="s">
+      <c r="G11" s="53" t="s">
+        <v>97</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="I11" s="36" t="s">
+      <c r="J11" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="J11" s="37">
+      <c r="K11" s="36">
         <v>3</v>
       </c>
-      <c r="K11" s="6"/>
-      <c r="L11" s="17" t="s">
+      <c r="L11" s="6"/>
+      <c r="M11" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="M11" s="6"/>
-      <c r="N11" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="O11" s="54" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="80" t="s">
+      <c r="N11" s="6"/>
+      <c r="O11" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P11" s="53" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="81" t="s">
+      <c r="B12" s="80" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="6"/>
-      <c r="D12" s="64" t="s">
+      <c r="D12" s="63" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="35" t="s">
+      <c r="G12" s="53" t="s">
+        <v>98</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="I12" s="36" t="s">
+      <c r="J12" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="37">
+      <c r="K12" s="36">
         <v>3</v>
       </c>
-      <c r="K12" s="6"/>
-      <c r="L12" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="M12" s="6"/>
-      <c r="N12" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="O12" s="54" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="80" t="s">
+      <c r="L12" s="6"/>
+      <c r="M12" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="N12" s="6"/>
+      <c r="O12" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P12" s="53" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="81" t="s">
+      <c r="B13" s="80" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="6"/>
-      <c r="D13" s="64" t="s">
+      <c r="D13" s="63" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="J13" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="K13" s="6"/>
-      <c r="L13" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="M13" s="6"/>
-      <c r="N13" s="35" t="s">
+      <c r="F13" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" s="6"/>
+      <c r="M13" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="N13" s="6"/>
+      <c r="O13" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="O13" s="54" t="s">
+      <c r="P13" s="53" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="80" t="s">
+    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="81" t="s">
+      <c r="B14" s="80" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="6"/>
-      <c r="D14" s="64" t="s">
+      <c r="D14" s="63" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="I14" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="J14" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="K14" s="6"/>
-      <c r="L14" s="17" t="s">
+      <c r="F14" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J14" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="K14" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="L14" s="6"/>
+      <c r="M14" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="M14" s="6"/>
-      <c r="N14" s="35" t="s">
+      <c r="N14" s="6"/>
+      <c r="O14" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="O14" s="54" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="80" t="s">
+      <c r="P14" s="53" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="80" t="s">
         <v>43</v>
       </c>
       <c r="C15" s="6"/>
-      <c r="D15" s="64" t="s">
+      <c r="D15" s="63" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="6"/>
-      <c r="F15" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="I15" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="J15" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="K15" s="6"/>
-      <c r="L15" s="17" t="s">
+      <c r="F15" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J15" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" s="6"/>
+      <c r="M15" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="M15" s="6"/>
-      <c r="N15" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="O15" s="54" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q15" s="91" t="s">
+      <c r="N15" s="6"/>
+      <c r="O15" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P15" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="R15" s="89" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="76"/>
-      <c r="B16" s="77"/>
-      <c r="D16" s="62"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="51"/>
-    </row>
-    <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="82" t="s">
+    <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="75"/>
+      <c r="B16" s="76"/>
+      <c r="D16" s="61"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="50"/>
+    </row>
+    <row r="17" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="83" t="s">
+      <c r="B17" s="82" t="s">
         <v>76</v>
       </c>
       <c r="C17" s="5"/>
-      <c r="D17" s="65" t="s">
+      <c r="D17" s="64" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="I17" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="J17" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="M17" s="5"/>
-      <c r="N17" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="O17" s="55" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="82" t="s">
+      <c r="G17" s="54" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" s="5"/>
+      <c r="I17" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="K17" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="L17" s="5"/>
+      <c r="M17" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N17" s="5"/>
+      <c r="O17" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="P17" s="54" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="83" t="s">
+      <c r="B18" s="82" t="s">
         <v>77</v>
       </c>
       <c r="C18" s="5"/>
-      <c r="D18" s="65" t="s">
+      <c r="D18" s="64" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="5"/>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="I18" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="J18" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="K18" s="5"/>
-      <c r="L18" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="M18" s="5"/>
-      <c r="N18" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="O18" s="55" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="82" t="s">
+      <c r="G18" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="H18" s="5"/>
+      <c r="I18" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="J18" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="K18" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="L18" s="5"/>
+      <c r="M18" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N18" s="5"/>
+      <c r="O18" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="P18" s="54" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="83" t="s">
+      <c r="B19" s="82" t="s">
         <v>78</v>
       </c>
       <c r="C19" s="5"/>
-      <c r="D19" s="65" t="s">
+      <c r="D19" s="64" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="I19" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="J19" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="K19" s="5"/>
-      <c r="L19" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="M19" s="5"/>
-      <c r="N19" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="O19" s="55" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="82" t="s">
+      <c r="G19" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="H19" s="5"/>
+      <c r="I19" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="J19" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="K19" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="L19" s="5"/>
+      <c r="M19" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N19" s="5"/>
+      <c r="O19" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="P19" s="54" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="83" t="s">
+      <c r="B20" s="82" t="s">
         <v>79</v>
       </c>
       <c r="C20" s="5"/>
-      <c r="D20" s="65" t="s">
+      <c r="D20" s="64" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="5"/>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="I20" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="J20" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="K20" s="5"/>
-      <c r="L20" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="M20" s="5"/>
-      <c r="N20" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="O20" s="55" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="82" t="s">
+      <c r="G20" s="54" t="s">
+        <v>102</v>
+      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="J20" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="K20" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="L20" s="5"/>
+      <c r="M20" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N20" s="5"/>
+      <c r="O20" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="P20" s="54" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="83" t="s">
+      <c r="B21" s="82" t="s">
         <v>80</v>
       </c>
       <c r="C21" s="5"/>
-      <c r="D21" s="65" t="s">
+      <c r="D21" s="64" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="5"/>
-      <c r="F21" s="18" t="s">
+      <c r="F21" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="I21" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="J21" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="K21" s="5"/>
-      <c r="L21" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="M21" s="5"/>
-      <c r="N21" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="O21" s="55" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="82" t="s">
+      <c r="G21" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="J21" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="K21" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="L21" s="5"/>
+      <c r="M21" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N21" s="5"/>
+      <c r="O21" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="P21" s="54" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="83" t="s">
+      <c r="B22" s="82" t="s">
         <v>81</v>
       </c>
       <c r="C22" s="5"/>
-      <c r="D22" s="65" t="s">
+      <c r="D22" s="64" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="5"/>
-      <c r="F22" s="18" t="s">
+      <c r="F22" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="G22" s="5"/>
-      <c r="H22" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="I22" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="J22" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="K22" s="5"/>
-      <c r="L22" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="M22" s="5"/>
-      <c r="N22" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="O22" s="55" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="82" t="s">
+      <c r="G22" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="H22" s="5"/>
+      <c r="I22" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="J22" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="K22" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="L22" s="5"/>
+      <c r="M22" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N22" s="5"/>
+      <c r="O22" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="P22" s="54" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="83" t="s">
+      <c r="B23" s="82" t="s">
         <v>82</v>
       </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="65" t="s">
+      <c r="D23" s="64" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="5"/>
-      <c r="F23" s="18" t="s">
+      <c r="F23" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="I23" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="J23" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="K23" s="5"/>
-      <c r="L23" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="M23" s="5"/>
-      <c r="N23" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="O23" s="55" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="82" t="s">
+      <c r="G23" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="H23" s="5"/>
+      <c r="I23" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="J23" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="K23" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="L23" s="5"/>
+      <c r="M23" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N23" s="5"/>
+      <c r="O23" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="P23" s="54" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="83" t="s">
+      <c r="B24" s="82" t="s">
         <v>83</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="D24" s="65" t="s">
+      <c r="D24" s="64" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="5"/>
-      <c r="F24" s="18" t="s">
+      <c r="F24" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="I24" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="J24" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="K24" s="5"/>
-      <c r="L24" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="M24" s="5"/>
-      <c r="N24" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="O24" s="55" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="82" t="s">
+      <c r="G24" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="H24" s="5"/>
+      <c r="I24" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="J24" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="K24" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="L24" s="5"/>
+      <c r="M24" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N24" s="5"/>
+      <c r="O24" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="P24" s="54" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="83" t="s">
+      <c r="B25" s="82" t="s">
         <v>84</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="65" t="s">
+      <c r="D25" s="64" t="s">
         <v>11</v>
       </c>
       <c r="E25" s="5"/>
-      <c r="F25" s="18" t="s">
+      <c r="F25" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="G25" s="5"/>
-      <c r="H25" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="I25" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="J25" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="K25" s="5"/>
-      <c r="L25" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="M25" s="5"/>
-      <c r="N25" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="O25" s="55" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="82" t="s">
+      <c r="G25" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="H25" s="5"/>
+      <c r="I25" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="J25" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="K25" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="L25" s="5"/>
+      <c r="M25" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N25" s="5"/>
+      <c r="O25" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="P25" s="54" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="83" t="s">
+      <c r="B26" s="82" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="65" t="s">
+      <c r="D26" s="64" t="s">
         <v>11</v>
       </c>
       <c r="E26" s="5"/>
-      <c r="F26" s="18" t="s">
+      <c r="F26" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="G26" s="5"/>
-      <c r="H26" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="I26" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="J26" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="K26" s="5"/>
-      <c r="L26" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="M26" s="5"/>
-      <c r="N26" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="O26" s="55" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="76"/>
-      <c r="B27" s="77"/>
-      <c r="D27" s="66"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="51"/>
-    </row>
-    <row r="28" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="84" t="s">
+      <c r="G26" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="H26" s="5"/>
+      <c r="I26" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="J26" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="K26" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="L26" s="5"/>
+      <c r="M26" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N26" s="5"/>
+      <c r="O26" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="P26" s="54" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="75"/>
+      <c r="B27" s="76"/>
+      <c r="D27" s="65"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="25"/>
+      <c r="P27" s="50"/>
+    </row>
+    <row r="28" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="85" t="s">
+      <c r="B28" s="84" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="3"/>
-      <c r="D28" s="67" t="s">
+      <c r="D28" s="66" t="s">
         <v>20</v>
       </c>
       <c r="E28" s="3"/>
-      <c r="F28" s="19" t="s">
+      <c r="F28" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="G28" s="3"/>
-      <c r="H28" s="41" t="s">
+      <c r="G28" s="55" t="s">
+        <v>110</v>
+      </c>
+      <c r="H28" s="3"/>
+      <c r="I28" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="I28" s="42" t="s">
+      <c r="J28" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="J28" s="43">
+      <c r="K28" s="42">
         <v>3</v>
       </c>
-      <c r="K28" s="3"/>
-      <c r="L28" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="M28" s="3"/>
-      <c r="N28" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="O28" s="56" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="84" t="s">
+      <c r="L28" s="3"/>
+      <c r="M28" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="N28" s="3"/>
+      <c r="O28" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="P28" s="55" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="85" t="s">
+      <c r="B29" s="84" t="s">
         <v>88</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="67" t="s">
+      <c r="D29" s="66" t="s">
         <v>20</v>
       </c>
       <c r="E29" s="3"/>
-      <c r="F29" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G29" s="3"/>
-      <c r="H29" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="I29" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="J29" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="K29" s="3"/>
-      <c r="L29" s="19" t="s">
+      <c r="F29" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="G29" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="H29" s="3"/>
+      <c r="I29" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="J29" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="K29" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="L29" s="3"/>
+      <c r="M29" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="M29" s="3"/>
-      <c r="N29" s="41" t="s">
+      <c r="N29" s="3"/>
+      <c r="O29" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="O29" s="56" t="s">
+      <c r="P29" s="55" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="84" t="s">
+    <row r="30" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="85" t="s">
+      <c r="B30" s="84" t="s">
         <v>21</v>
       </c>
       <c r="C30" s="3"/>
-      <c r="D30" s="67" t="s">
+      <c r="D30" s="66" t="s">
         <v>20</v>
       </c>
       <c r="E30" s="3"/>
-      <c r="F30" s="19" t="s">
+      <c r="F30" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="G30" s="3"/>
-      <c r="H30" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="I30" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="J30" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="K30" s="3"/>
-      <c r="L30" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="M30" s="3"/>
-      <c r="N30" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="O30" s="56" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="84" t="s">
+      <c r="G30" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="H30" s="3"/>
+      <c r="I30" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="J30" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="K30" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="L30" s="3"/>
+      <c r="M30" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="N30" s="3"/>
+      <c r="O30" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="P30" s="55" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="85" t="s">
+      <c r="B31" s="84" t="s">
         <v>22</v>
       </c>
       <c r="C31" s="3"/>
-      <c r="D31" s="67" t="s">
+      <c r="D31" s="66" t="s">
         <v>20</v>
       </c>
       <c r="E31" s="3"/>
-      <c r="F31" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G31" s="3"/>
-      <c r="H31" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="I31" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="J31" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="K31" s="3"/>
-      <c r="L31" s="19" t="s">
+      <c r="F31" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="G31" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="H31" s="3"/>
+      <c r="I31" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="J31" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="K31" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="L31" s="3"/>
+      <c r="M31" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="M31" s="3"/>
-      <c r="N31" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="O31" s="56" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q31" s="91" t="s">
+      <c r="N31" s="3"/>
+      <c r="O31" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="P31" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="R31" s="89" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="76"/>
-      <c r="B32" s="77"/>
-      <c r="D32" s="62"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="28"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="26"/>
-      <c r="O32" s="51"/>
-    </row>
-    <row r="33" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="86" t="s">
+    <row r="32" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="75"/>
+      <c r="B32" s="76"/>
+      <c r="D32" s="61"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="27"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="25"/>
+      <c r="P32" s="50"/>
+    </row>
+    <row r="33" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="87" t="s">
+      <c r="B33" s="86" t="s">
         <v>30</v>
       </c>
       <c r="C33" s="10"/>
-      <c r="D33" s="68" t="s">
+      <c r="D33" s="67" t="s">
         <v>29</v>
       </c>
       <c r="E33" s="10"/>
-      <c r="F33" s="20" t="s">
+      <c r="F33" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="G33" s="10"/>
-      <c r="H33" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="I33" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="J33" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="K33" s="10"/>
-      <c r="L33" s="21" t="s">
+      <c r="G33" s="92" t="s">
+        <v>112</v>
+      </c>
+      <c r="H33" s="10"/>
+      <c r="I33" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="J33" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="K33" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="L33" s="10"/>
+      <c r="M33" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="M33" s="10"/>
-      <c r="N33" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="O33" s="57" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="86" t="s">
+      <c r="N33" s="10"/>
+      <c r="O33" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="P33" s="56" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="87" t="s">
+      <c r="B34" s="86" t="s">
         <v>28</v>
       </c>
       <c r="C34" s="10"/>
-      <c r="D34" s="68" t="s">
+      <c r="D34" s="67" t="s">
         <v>29</v>
       </c>
       <c r="E34" s="10"/>
-      <c r="F34" s="21" t="s">
+      <c r="F34" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="G34" s="10"/>
-      <c r="H34" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="I34" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="J34" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="K34" s="10"/>
-      <c r="L34" s="21" t="s">
+      <c r="G34" s="56" t="s">
+        <v>113</v>
+      </c>
+      <c r="H34" s="10"/>
+      <c r="I34" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="J34" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="K34" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="L34" s="10"/>
+      <c r="M34" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="M34" s="10"/>
-      <c r="N34" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="O34" s="57" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="88" t="s">
+      <c r="N34" s="10"/>
+      <c r="O34" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="P34" s="56" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="89" t="s">
+      <c r="B35" s="88" t="s">
         <v>31</v>
       </c>
       <c r="C35" s="10"/>
-      <c r="D35" s="69" t="s">
+      <c r="D35" s="68" t="s">
         <v>29</v>
       </c>
       <c r="E35" s="10"/>
-      <c r="F35" s="22" t="s">
+      <c r="F35" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="G35" s="10"/>
-      <c r="H35" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="I35" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="J35" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="K35" s="10"/>
-      <c r="L35" s="22" t="s">
+      <c r="G35" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="H35" s="10"/>
+      <c r="I35" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="J35" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="K35" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="L35" s="10"/>
+      <c r="M35" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="M35" s="10"/>
-      <c r="N35" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="O35" s="58" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N35" s="10"/>
+      <c r="O35" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="P35" s="57" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="60" orientation="landscape" r:id="rId1"/>

</xml_diff>